<commit_message>
Implemented keydefmap extraction of XLIFF files including selection of source vs target based on 'patharea'.
</commit_message>
<xml_diff>
--- a/src/test/resources/Techdata1.xlsx
+++ b/src/test/resources/Techdata1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="28200" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="28200" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="First sheet" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Just</t>
   </si>
@@ -104,6 +104,9 @@
   <si>
     <t>Multi
 Line</t>
+  </si>
+  <si>
+    <t>Key</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -448,6 +451,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -521,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>